<commit_message>
first gui version with problem of setting new ms2window value
</commit_message>
<xml_diff>
--- a/ExcelProcessor/lipid.xlsx
+++ b/ExcelProcessor/lipid.xlsx
@@ -8,6 +8,7 @@
   <s:sheets>
     <s:sheet name="Sheet-1" sheetId="1" r:id="rId1"/>
     <s:sheet name="Sheet-2" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Sheet-3" sheetId="3" r:id="rId3"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Lipid</t>
   </si>
@@ -207,6 +208,30 @@
   </si>
   <si>
     <t>Area6/Area3</t>
+  </si>
+  <si>
+    <t>10.1/10.5</t>
+  </si>
+  <si>
+    <t>10.1/10.2/10.5</t>
+  </si>
+  <si>
+    <t>10.45/11.64</t>
+  </si>
+  <si>
+    <t>10.55</t>
+  </si>
+  <si>
+    <t>10.3/10.4</t>
+  </si>
+  <si>
+    <t>10.1/10.2</t>
+  </si>
+  <si>
+    <t>10.8/10.3/10.4</t>
+  </si>
+  <si>
+    <t>10.8/10.3</t>
   </si>
 </sst>
 </file>
@@ -1550,14 +1575,2010 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>